<commit_message>
Scripts DML e DQL Concluídos
</commit_message>
<xml_diff>
--- a/SP-Medical-Group/Modelo Físico.xlsx
+++ b/SP-Medical-Group/Modelo Físico.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIC\Desktop\Andre\Senai_sprint1_bd\SP-Medical-Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\Andre\Senai_sprint1_bd\SP-Medical-Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C57E4F-E320-4CC9-BBDB-04CE1EE3E8CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7A5BED-21AF-4F9C-97BD-97B1FF3F0138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{53AF2A13-9DFC-4EF9-A1F6-D35D99848663}"/>
   </bookViews>
@@ -465,26 +465,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,41 +488,53 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DB3900-8893-43EB-B24D-717962F93EE5}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,21 +873,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="23"/>
+      <c r="D1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="24"/>
+      <c r="G1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -896,25 +896,25 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -925,25 +925,25 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -954,10 +954,10 @@
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -968,641 +968,641 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>4</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>5</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>6</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="7">
         <v>1</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="7">
         <v>2</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>7</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="7">
         <v>2</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="7">
         <v>2</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>8</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="11">
-        <v>3</v>
-      </c>
-      <c r="I10" s="11">
+      <c r="H10" s="7">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7">
         <v>2</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>9</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="7">
         <v>4</v>
       </c>
-      <c r="I11" s="11">
-        <v>3</v>
-      </c>
-      <c r="J11" s="14" t="s">
+      <c r="I11" s="7">
+        <v>3</v>
+      </c>
+      <c r="J11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>10</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="7">
         <v>5</v>
       </c>
-      <c r="I12" s="11">
-        <v>3</v>
-      </c>
-      <c r="J12" s="14" t="s">
+      <c r="I12" s="7">
+        <v>3</v>
+      </c>
+      <c r="J12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="9" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>11</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="7">
         <v>6</v>
       </c>
-      <c r="I13" s="11">
-        <v>3</v>
-      </c>
-      <c r="J13" s="14" t="s">
+      <c r="I13" s="7">
+        <v>3</v>
+      </c>
+      <c r="J13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>12</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="7">
         <v>7</v>
       </c>
-      <c r="I14" s="11">
-        <v>3</v>
-      </c>
-      <c r="J14" s="14" t="s">
+      <c r="I14" s="7">
+        <v>3</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>13</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="7">
         <v>8</v>
       </c>
-      <c r="I15" s="11">
-        <v>3</v>
-      </c>
-      <c r="J15" s="14" t="s">
+      <c r="I15" s="7">
+        <v>3</v>
+      </c>
+      <c r="J15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K15" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>14</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="7">
         <v>9</v>
       </c>
-      <c r="I16" s="11">
-        <v>3</v>
-      </c>
-      <c r="J16" s="14" t="s">
+      <c r="I16" s="7">
+        <v>3</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>15</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="7">
         <v>10</v>
       </c>
-      <c r="I17" s="11">
-        <v>3</v>
-      </c>
-      <c r="J17" s="14" t="s">
+      <c r="I17" s="7">
+        <v>3</v>
+      </c>
+      <c r="J17" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="13" t="s">
+      <c r="K17" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>16</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>17</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="H21" s="20" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="H21" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="19" t="s">
+      <c r="L22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="M22" s="19" t="s">
+      <c r="M22" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="N22" s="19" t="s">
+      <c r="N22" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+      <c r="A23" s="12">
         <v>1</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="12">
         <v>1</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="12">
         <v>1</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="21">
+      <c r="H23" s="15">
         <v>1</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I23" s="15">
         <v>4</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J23" s="16">
         <v>30602</v>
       </c>
-      <c r="K23" s="23" t="s">
+      <c r="K23" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="L23" s="23" t="s">
+      <c r="L23" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="M23" s="23">
+      <c r="M23" s="17">
         <v>94839859000</v>
       </c>
-      <c r="N23" s="24" t="s">
+      <c r="N23" s="18" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="A24" s="12">
         <v>2</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="12">
         <v>2</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="12">
         <v>17</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="12">
         <v>1</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="21">
+      <c r="H24" s="15">
         <v>2</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I24" s="15">
         <v>5</v>
       </c>
-      <c r="J24" s="22">
+      <c r="J24" s="16">
         <v>37095</v>
       </c>
-      <c r="K24" s="23" t="s">
+      <c r="K24" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="17">
         <v>73556944057</v>
       </c>
-      <c r="N24" s="25" t="s">
+      <c r="N24" s="19" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
-        <v>3</v>
-      </c>
-      <c r="B25" s="17">
-        <v>3</v>
-      </c>
-      <c r="C25" s="17">
+      <c r="A25" s="12">
+        <v>3</v>
+      </c>
+      <c r="B25" s="12">
+        <v>3</v>
+      </c>
+      <c r="C25" s="12">
         <v>16</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="12">
         <v>1</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="21">
-        <v>3</v>
-      </c>
-      <c r="I25" s="21">
+      <c r="H25" s="15">
+        <v>3</v>
+      </c>
+      <c r="I25" s="15">
         <v>6</v>
       </c>
-      <c r="J25" s="22">
+      <c r="J25" s="16">
         <v>28773</v>
       </c>
-      <c r="K25" s="23" t="s">
+      <c r="K25" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="L25" s="23" t="s">
+      <c r="L25" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="M25" s="23">
+      <c r="M25" s="17">
         <v>16839338002</v>
       </c>
-      <c r="N25" s="25" t="s">
+      <c r="N25" s="19" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H26" s="21">
+      <c r="H26" s="15">
         <v>4</v>
       </c>
-      <c r="I26" s="21">
+      <c r="I26" s="15">
         <v>7</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J26" s="16">
         <v>31333</v>
       </c>
-      <c r="K26" s="23" t="s">
+      <c r="K26" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="L26" s="23" t="s">
+      <c r="L26" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="M26" s="23">
+      <c r="M26" s="17">
         <v>14332654765</v>
       </c>
-      <c r="N26" s="25" t="s">
+      <c r="N26" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H27" s="21">
+      <c r="H27" s="15">
         <v>5</v>
       </c>
-      <c r="I27" s="21">
+      <c r="I27" s="15">
         <v>8</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J27" s="16">
         <v>27633</v>
       </c>
-      <c r="K27" s="23" t="s">
+      <c r="K27" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="L27" s="23" t="s">
+      <c r="L27" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M27" s="23">
+      <c r="M27" s="17">
         <v>91305348010</v>
       </c>
-      <c r="N27" s="25" t="s">
+      <c r="N27" s="19" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H28" s="21">
+      <c r="H28" s="15">
         <v>6</v>
       </c>
-      <c r="I28" s="21">
+      <c r="I28" s="15">
         <v>9</v>
       </c>
-      <c r="J28" s="22">
+      <c r="J28" s="16">
         <v>26379</v>
       </c>
-      <c r="K28" s="23" t="s">
+      <c r="K28" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="L28" s="23" t="s">
+      <c r="L28" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="17">
         <v>79799299004</v>
       </c>
-      <c r="N28" s="25" t="s">
+      <c r="N28" s="19" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H29" s="21">
+      <c r="H29" s="15">
         <v>7</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I29" s="15">
         <v>10</v>
       </c>
-      <c r="J29" s="22">
+      <c r="J29" s="16">
         <v>43164</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="23" t="s">
+      <c r="K29" s="15"/>
+      <c r="L29" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="M29" s="23">
+      <c r="M29" s="17">
         <v>13771913039</v>
       </c>
-      <c r="N29" s="25" t="s">
+      <c r="N29" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="20" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="27">
+      <c r="A32" s="20">
         <v>1</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="20">
         <v>7</v>
       </c>
-      <c r="C32" s="27">
-        <v>3</v>
-      </c>
-      <c r="D32" s="27" t="s">
+      <c r="C32" s="20">
+        <v>3</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="27">
+      <c r="A33" s="20">
         <v>2</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="20">
         <v>2</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="20">
         <v>2</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="20" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="27">
-        <v>3</v>
-      </c>
-      <c r="B34" s="27">
-        <v>3</v>
-      </c>
-      <c r="C34" s="27">
+      <c r="A34" s="20">
+        <v>3</v>
+      </c>
+      <c r="B34" s="20">
+        <v>3</v>
+      </c>
+      <c r="C34" s="20">
         <v>2</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27">
+      <c r="A35" s="20">
         <v>4</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="20">
         <v>2</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="20">
         <v>2</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
+      <c r="A36" s="20">
         <v>5</v>
       </c>
-      <c r="B36" s="27">
+      <c r="B36" s="20">
         <v>4</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="20">
         <v>1</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="20" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
+      <c r="A37" s="20">
         <v>6</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="20">
         <v>7</v>
       </c>
-      <c r="C37" s="27">
-        <v>3</v>
-      </c>
-      <c r="D37" s="27" t="s">
+      <c r="C37" s="20">
+        <v>3</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E37" s="28"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
+      <c r="A38" s="20">
         <v>7</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="20">
         <v>4</v>
       </c>
-      <c r="C38" s="27">
+      <c r="C38" s="20">
         <v>1</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="20" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Scripts DML e DDL concluídos
</commit_message>
<xml_diff>
--- a/SP-Medical-Group/Modelo Físico.xlsx
+++ b/SP-Medical-Group/Modelo Físico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\Andre\Senai_sprint1_bd\SP-Medical-Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7A5BED-21AF-4F9C-97BD-97B1FF3F0138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9756853-B69E-45A4-B195-520D94AA2049}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{53AF2A13-9DFC-4EF9-A1F6-D35D99848663}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t>tipoUsuario</t>
   </si>
@@ -307,13 +307,19 @@
   </si>
   <si>
     <t>Agendada</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>adm@adm.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +358,14 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="16">
@@ -472,7 +486,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -533,6 +546,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -850,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DB3900-8893-43EB-B24D-717962F93EE5}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,21 +889,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="D1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="G1" s="25" t="s">
+      <c r="E1" s="23"/>
+      <c r="G1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -982,12 +998,12 @@
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7" s="4">
@@ -996,639 +1012,656 @@
       <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D8" s="4">
-        <v>6</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="H8" s="6">
         <v>1</v>
       </c>
-      <c r="I8" s="7">
-        <v>2</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>39</v>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="7">
+        <v>14</v>
+      </c>
+      <c r="H9" s="6">
         <v>2</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>2</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>41</v>
+      <c r="J9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="7">
-        <v>3</v>
-      </c>
-      <c r="I10" s="7">
+        <v>15</v>
+      </c>
+      <c r="H10" s="6">
+        <v>3</v>
+      </c>
+      <c r="I10" s="6">
         <v>2</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>43</v>
+      <c r="J10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="7">
+        <v>17</v>
+      </c>
+      <c r="H11" s="6">
         <v>4</v>
       </c>
-      <c r="I11" s="7">
-        <v>3</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>45</v>
+      <c r="I11" s="6">
+        <v>2</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="7">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6">
         <v>5</v>
       </c>
-      <c r="I12" s="7">
-        <v>3</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>47</v>
+      <c r="I12" s="6">
+        <v>3</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="7">
+        <v>18</v>
+      </c>
+      <c r="H13" s="6">
         <v>6</v>
       </c>
-      <c r="I13" s="7">
-        <v>3</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>49</v>
+      <c r="I13" s="6">
+        <v>3</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="7">
+        <v>19</v>
+      </c>
+      <c r="H14" s="6">
         <v>7</v>
       </c>
-      <c r="I14" s="7">
-        <v>3</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>54</v>
+      <c r="I14" s="6">
+        <v>3</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="7">
+        <v>20</v>
+      </c>
+      <c r="H15" s="6">
         <v>8</v>
       </c>
-      <c r="I15" s="7">
-        <v>3</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>55</v>
+      <c r="I15" s="6">
+        <v>3</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="7">
+        <v>21</v>
+      </c>
+      <c r="H16" s="6">
         <v>9</v>
       </c>
-      <c r="I16" s="7">
-        <v>3</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>56</v>
+      <c r="I16" s="6">
+        <v>3</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D17" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="7">
+        <v>22</v>
+      </c>
+      <c r="H17" s="6">
         <v>10</v>
       </c>
-      <c r="I17" s="7">
-        <v>3</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>57</v>
+      <c r="I17" s="6">
+        <v>3</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D18" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="H18" s="6">
+        <v>11</v>
+      </c>
+      <c r="I18" s="6">
+        <v>3</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D19" s="4">
+        <v>16</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D20" s="4">
         <v>17</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="H21" s="28" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="H22" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H23" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J23" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K23" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="14" t="s">
+      <c r="L23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M23" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="N22" s="14" t="s">
+      <c r="N23" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
         <v>1</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B24" s="11">
+        <v>2</v>
+      </c>
+      <c r="C24" s="11">
+        <v>2</v>
+      </c>
+      <c r="D24" s="11">
         <v>1</v>
       </c>
-      <c r="C23" s="12">
+      <c r="E24" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="14">
+        <v>1</v>
+      </c>
+      <c r="I24" s="14">
+        <v>4</v>
+      </c>
+      <c r="J24" s="15">
+        <v>30602</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="M24" s="16">
+        <v>94839859000</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
         <v>2</v>
       </c>
-      <c r="D23" s="12">
+      <c r="B25" s="11">
+        <v>3</v>
+      </c>
+      <c r="C25" s="11">
+        <v>17</v>
+      </c>
+      <c r="D25" s="11">
         <v>1</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H23" s="15">
+      <c r="E25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="14">
+        <v>2</v>
+      </c>
+      <c r="I25" s="14">
+        <v>5</v>
+      </c>
+      <c r="J25" s="15">
+        <v>37095</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M25" s="16">
+        <v>73556944057</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>3</v>
+      </c>
+      <c r="B26" s="11">
+        <v>4</v>
+      </c>
+      <c r="C26" s="11">
+        <v>16</v>
+      </c>
+      <c r="D26" s="11">
         <v>1</v>
       </c>
-      <c r="I23" s="15">
+      <c r="E26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="14">
+        <v>3</v>
+      </c>
+      <c r="I26" s="14">
+        <v>6</v>
+      </c>
+      <c r="J26" s="15">
+        <v>28773</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="M26" s="16">
+        <v>16839338002</v>
+      </c>
+      <c r="N26" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H27" s="14">
         <v>4</v>
       </c>
-      <c r="J23" s="16">
-        <v>30602</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="M23" s="17">
-        <v>94839859000</v>
-      </c>
-      <c r="N23" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+      <c r="I27" s="14">
+        <v>7</v>
+      </c>
+      <c r="J27" s="15">
+        <v>31333</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="M27" s="16">
+        <v>14332654765</v>
+      </c>
+      <c r="N27" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H28" s="14">
+        <v>5</v>
+      </c>
+      <c r="I28" s="14">
+        <v>8</v>
+      </c>
+      <c r="J28" s="15">
+        <v>27633</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M28" s="16">
+        <v>91305348010</v>
+      </c>
+      <c r="N28" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H29" s="14">
+        <v>6</v>
+      </c>
+      <c r="I29" s="14">
+        <v>9</v>
+      </c>
+      <c r="J29" s="15">
+        <v>26379</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="M29" s="16">
+        <v>79799299004</v>
+      </c>
+      <c r="N29" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H30" s="14">
+        <v>7</v>
+      </c>
+      <c r="I30" s="14">
+        <v>10</v>
+      </c>
+      <c r="J30" s="15">
+        <v>43164</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="M30" s="16">
+        <v>13771913039</v>
+      </c>
+      <c r="N30" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="19">
+        <v>1</v>
+      </c>
+      <c r="B33" s="19">
+        <v>7</v>
+      </c>
+      <c r="C33" s="19">
+        <v>3</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="19">
         <v>2</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B34" s="19">
         <v>2</v>
       </c>
-      <c r="C24" s="12">
-        <v>17</v>
-      </c>
-      <c r="D24" s="12">
+      <c r="C34" s="19">
+        <v>2</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="19">
+        <v>3</v>
+      </c>
+      <c r="B35" s="19">
+        <v>3</v>
+      </c>
+      <c r="C35" s="19">
+        <v>2</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="19">
+        <v>4</v>
+      </c>
+      <c r="B36" s="19">
+        <v>2</v>
+      </c>
+      <c r="C36" s="19">
+        <v>2</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="19">
+        <v>5</v>
+      </c>
+      <c r="B37" s="19">
+        <v>4</v>
+      </c>
+      <c r="C37" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="H24" s="15">
-        <v>2</v>
-      </c>
-      <c r="I24" s="15">
-        <v>5</v>
-      </c>
-      <c r="J24" s="16">
-        <v>37095</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="L24" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="M24" s="17">
-        <v>73556944057</v>
-      </c>
-      <c r="N24" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>3</v>
-      </c>
-      <c r="B25" s="12">
-        <v>3</v>
-      </c>
-      <c r="C25" s="12">
-        <v>16</v>
-      </c>
-      <c r="D25" s="12">
+      <c r="D37" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="19">
+        <v>6</v>
+      </c>
+      <c r="B38" s="19">
+        <v>7</v>
+      </c>
+      <c r="C38" s="19">
+        <v>3</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="19">
+        <v>7</v>
+      </c>
+      <c r="B39" s="19">
+        <v>4</v>
+      </c>
+      <c r="C39" s="19">
         <v>1</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="15">
-        <v>3</v>
-      </c>
-      <c r="I25" s="15">
-        <v>6</v>
-      </c>
-      <c r="J25" s="16">
-        <v>28773</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="M25" s="17">
-        <v>16839338002</v>
-      </c>
-      <c r="N25" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H26" s="15">
-        <v>4</v>
-      </c>
-      <c r="I26" s="15">
-        <v>7</v>
-      </c>
-      <c r="J26" s="16">
-        <v>31333</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="L26" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="M26" s="17">
-        <v>14332654765</v>
-      </c>
-      <c r="N26" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H27" s="15">
-        <v>5</v>
-      </c>
-      <c r="I27" s="15">
-        <v>8</v>
-      </c>
-      <c r="J27" s="16">
-        <v>27633</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="L27" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="M27" s="17">
-        <v>91305348010</v>
-      </c>
-      <c r="N27" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H28" s="15">
-        <v>6</v>
-      </c>
-      <c r="I28" s="15">
-        <v>9</v>
-      </c>
-      <c r="J28" s="16">
-        <v>26379</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="L28" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="M28" s="17">
-        <v>79799299004</v>
-      </c>
-      <c r="N28" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H29" s="15">
-        <v>7</v>
-      </c>
-      <c r="I29" s="15">
-        <v>10</v>
-      </c>
-      <c r="J29" s="16">
-        <v>43164</v>
-      </c>
-      <c r="K29" s="15"/>
-      <c r="L29" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="M29" s="17">
-        <v>13771913039</v>
-      </c>
-      <c r="N29" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
-        <v>1</v>
-      </c>
-      <c r="B32" s="20">
-        <v>7</v>
-      </c>
-      <c r="C32" s="20">
-        <v>3</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
-        <v>2</v>
-      </c>
-      <c r="B33" s="20">
-        <v>2</v>
-      </c>
-      <c r="C33" s="20">
-        <v>2</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
-        <v>3</v>
-      </c>
-      <c r="B34" s="20">
-        <v>3</v>
-      </c>
-      <c r="C34" s="20">
-        <v>2</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
-        <v>4</v>
-      </c>
-      <c r="B35" s="20">
-        <v>2</v>
-      </c>
-      <c r="C35" s="20">
-        <v>2</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
-        <v>5</v>
-      </c>
-      <c r="B36" s="20">
-        <v>4</v>
-      </c>
-      <c r="C36" s="20">
-        <v>1</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
-        <v>6</v>
-      </c>
-      <c r="B37" s="20">
-        <v>7</v>
-      </c>
-      <c r="C37" s="20">
-        <v>3</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="21"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
-        <v>7</v>
-      </c>
-      <c r="B38" s="20">
-        <v>4</v>
-      </c>
-      <c r="C38" s="20">
-        <v>1</v>
-      </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="19" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="H21:N21"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="H22:N22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId1" display="mailto:ricardo.lemos@spmedicalgroup.com.br" xr:uid="{83FC85F4-8823-4F66-B3F5-1AC8B5C72F16}"/>
-    <hyperlink ref="K9" r:id="rId2" display="mailto:roberto.possarle@spmedicalgroup.com.br" xr:uid="{2A50C302-D322-49ED-B260-208A44E111DF}"/>
-    <hyperlink ref="K10" r:id="rId3" display="mailto:helena.souza@spmedicalgroup.com.br" xr:uid="{73E29DEB-4227-404A-BBAB-2BC1BE830BD7}"/>
-    <hyperlink ref="K11" r:id="rId4" display="mailto:ligia@gmail.com" xr:uid="{6CC70BF3-2F8B-436A-90E4-E92880886D74}"/>
-    <hyperlink ref="K12" r:id="rId5" display="mailto:alexandre@gmail.com" xr:uid="{5BCD5423-C5F8-4982-841E-7A2B952A3608}"/>
-    <hyperlink ref="K13" r:id="rId6" display="mailto:fernando@gmail.com" xr:uid="{5AD7D4F5-D9E9-4E6E-A6BC-5D818F7989C4}"/>
-    <hyperlink ref="K14" r:id="rId7" display="mailto:henrique@gmail.com" xr:uid="{8E678CE2-0B4E-4209-BCCA-957B3E6CDB8C}"/>
-    <hyperlink ref="K15" r:id="rId8" display="mailto:joao@hotmail.com" xr:uid="{0FEF5675-C0B2-488C-9BE0-7F04DFB9C992}"/>
-    <hyperlink ref="K16" r:id="rId9" display="mailto:bruno@gmail.com" xr:uid="{1C4E0D04-EDF8-49F9-90D7-F7A405B4A1D8}"/>
-    <hyperlink ref="K17" r:id="rId10" display="mailto:mariana@outlook.com" xr:uid="{DB92A93A-2E1B-40F5-B736-C9DC640B572D}"/>
+    <hyperlink ref="K9" r:id="rId1" display="mailto:ricardo.lemos@spmedicalgroup.com.br" xr:uid="{83FC85F4-8823-4F66-B3F5-1AC8B5C72F16}"/>
+    <hyperlink ref="K10" r:id="rId2" display="mailto:roberto.possarle@spmedicalgroup.com.br" xr:uid="{2A50C302-D322-49ED-B260-208A44E111DF}"/>
+    <hyperlink ref="K11" r:id="rId3" display="mailto:helena.souza@spmedicalgroup.com.br" xr:uid="{73E29DEB-4227-404A-BBAB-2BC1BE830BD7}"/>
+    <hyperlink ref="K12" r:id="rId4" display="mailto:ligia@gmail.com" xr:uid="{6CC70BF3-2F8B-436A-90E4-E92880886D74}"/>
+    <hyperlink ref="K13" r:id="rId5" display="mailto:alexandre@gmail.com" xr:uid="{5BCD5423-C5F8-4982-841E-7A2B952A3608}"/>
+    <hyperlink ref="K14" r:id="rId6" display="mailto:fernando@gmail.com" xr:uid="{5AD7D4F5-D9E9-4E6E-A6BC-5D818F7989C4}"/>
+    <hyperlink ref="K15" r:id="rId7" display="mailto:henrique@gmail.com" xr:uid="{8E678CE2-0B4E-4209-BCCA-957B3E6CDB8C}"/>
+    <hyperlink ref="K16" r:id="rId8" display="mailto:joao@hotmail.com" xr:uid="{0FEF5675-C0B2-488C-9BE0-7F04DFB9C992}"/>
+    <hyperlink ref="K17" r:id="rId9" display="mailto:bruno@gmail.com" xr:uid="{1C4E0D04-EDF8-49F9-90D7-F7A405B4A1D8}"/>
+    <hyperlink ref="K18" r:id="rId10" display="mailto:mariana@outlook.com" xr:uid="{DB92A93A-2E1B-40F5-B736-C9DC640B572D}"/>
+    <hyperlink ref="K8" r:id="rId11" xr:uid="{9EA7EF3C-F393-4D30-A433-23E6BAA895D1}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>